<commit_message>
Atualiza todos os resources para "active"
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BRCodigoSerialMedicamento.xlsx
+++ b/docs/StructureDefinition-BRCodigoSerialMedicamento.xlsx
@@ -48,7 +48,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-18T12:40:46-03:00</t>
+    <t>2024-01-18T17:12:33-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>